<commit_message>
Exception class setup, further Listeners and factory classes setup
</commit_message>
<xml_diff>
--- a/selenium-framework/src/test/resources/excel/TestData.xlsx
+++ b/selenium-framework/src/test/resources/excel/TestData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="3820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="3820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>TestName</t>
   </si>
@@ -50,6 +50,27 @@
   </si>
   <si>
     <t>test2</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Aman123</t>
+  </si>
+  <si>
+    <t>Saba</t>
+  </si>
+  <si>
+    <t>Saba123</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -196,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -228,11 +249,155 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -410,14 +575,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:E3"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="TestName" dataDxfId="4"/>
-    <tableColumn id="2" name="TestDescription" dataDxfId="3"/>
-    <tableColumn id="3" name="Execute" dataDxfId="2"/>
-    <tableColumn id="4" name="Priority" dataDxfId="1"/>
-    <tableColumn id="5" name="Count" dataDxfId="0"/>
+    <tableColumn id="1" name="TestName" dataDxfId="13"/>
+    <tableColumn id="2" name="TestDescription" dataDxfId="12"/>
+    <tableColumn id="3" name="Execute" dataDxfId="11"/>
+    <tableColumn id="4" name="Priority" dataDxfId="10"/>
+    <tableColumn id="5" name="Count" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="TestName" dataDxfId="3"/>
+    <tableColumn id="2" name="Execute" dataDxfId="2"/>
+    <tableColumn id="3" name="Username" dataDxfId="1"/>
+    <tableColumn id="4" name="Password" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -688,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,4 +936,78 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>